<commit_message>
after burn flash, the first time is zigbee network config
</commit_message>
<xml_diff>
--- a/zigbee_xbr/DOC/flash分配.xlsx
+++ b/zigbee_xbr/DOC/flash分配.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>全局变量</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -139,6 +139,21 @@
   </si>
   <si>
     <t>不开雷达时的亮度值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x2F81</t>
+  </si>
+  <si>
+    <t>u8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>zigbee_join_cnt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>烧写后第一次上电为配网</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -541,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -552,7 +567,7 @@
     <col min="1" max="1" width="11.73046875" style="2" customWidth="1"/>
     <col min="2" max="2" width="19.19921875" style="2" customWidth="1"/>
     <col min="3" max="3" width="10.9296875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="21.73046875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="22.796875" style="2" customWidth="1"/>
     <col min="5" max="5" width="21" style="2" customWidth="1"/>
     <col min="6" max="16384" width="9.06640625" style="2"/>
   </cols>
@@ -706,6 +721,23 @@
       </c>
       <c r="E9" s="1" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add some flash access
</commit_message>
<xml_diff>
--- a/zigbee_xbr/DOC/flash分配.xlsx
+++ b/zigbee_xbr/DOC/flash分配.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
   <si>
     <t>全局变量</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -154,6 +154,45 @@
   </si>
   <si>
     <t>烧写后第一次上电为配网</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>u8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x2F08</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>联动标志位</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Linkage_flag</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x2F09</t>
+  </si>
+  <si>
+    <t>0x2F0A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SWITCHflag2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>开关灯</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>all_day_micro_light_enable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>全天伴亮</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -556,16 +595,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="11.73046875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="19.19921875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="27.86328125" style="2" customWidth="1"/>
     <col min="3" max="3" width="10.9296875" style="2" customWidth="1"/>
     <col min="4" max="4" width="22.796875" style="2" customWidth="1"/>
     <col min="5" max="5" width="21" style="2" customWidth="1"/>
@@ -711,16 +750,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -728,15 +767,66 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
first working version for warm and cold light
</commit_message>
<xml_diff>
--- a/zigbee_xbr/DOC/flash分配.xlsx
+++ b/zigbee_xbr/DOC/flash分配.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
   <si>
     <t>全局变量</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -193,6 +193,22 @@
   </si>
   <si>
     <t>全天伴亮</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>u8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>temper_value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>冷暖选择值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x2F0B</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -595,10 +611,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -801,16 +817,16 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>10</v>
+        <v>45</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>27</v>
+        <v>47</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>22</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -818,15 +834,32 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E14" s="1" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adapt a log change from the wifi-bt warm-cold product branch
</commit_message>
<xml_diff>
--- a/zigbee_xbr/DOC/flash分配.xlsx
+++ b/zigbee_xbr/DOC/flash分配.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="53">
   <si>
     <t>全局变量</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -46,14 +46,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>地址</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0x2F00~0x2F01</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>LIGHT_TH</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -62,18 +54,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0x2F02</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>DELAY_NUM</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0x2F03~0x2F04</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>lightvalue</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -82,34 +66,18 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0x2F05</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>lowlightDELAY_NUM</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0x2F06</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>SWITCHfXBR</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0x2F07</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>resetbtcnt</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0x2F80</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>光照门限</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -142,9 +110,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0x2F81</t>
-  </si>
-  <si>
     <t>u8</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -161,10 +126,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0x2F08</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>联动标志位</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -173,13 +134,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0x2F09</t>
-  </si>
-  <si>
-    <t>0x2F0A</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>SWITCHflag2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -208,8 +162,70 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>0x2F0B</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>偏移地址</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x00~0x01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x02</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x03~0x04</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x05</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x06</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x07</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x08</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x09</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>扇区基地址</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>USER_PARAMETER_START_SECTOR_ADDRESS0</t>
+  </si>
+  <si>
+    <t>USER_PARAMETER_START_SECTOR_ADDRESS0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>USER_PARAMETER_START_SECTOR_ADDRESS1</t>
   </si>
 </sst>
 </file>
@@ -241,7 +257,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -264,39 +280,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -306,10 +296,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -611,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -624,10 +611,11 @@
     <col min="3" max="3" width="10.9296875" style="2" customWidth="1"/>
     <col min="4" max="4" width="22.796875" style="2" customWidth="1"/>
     <col min="5" max="5" width="21" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="9.06640625" style="2"/>
+    <col min="6" max="6" width="38.86328125" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="9.06640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -641,10 +629,13 @@
         <v>6</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
+        <v>36</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -655,212 +646,251 @@
         <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>37</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>38</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>39</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>40</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E6" s="4"/>
-    </row>
-    <row r="7" spans="1:5">
+        <v>22</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>41</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>42</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>43</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>44</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>45</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="F12" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>47</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>31</v>
+        <v>48</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>